<commit_message>
Created Excel data provider Created TestNG Data Provider Created Test Case flow Created locater using page factory Created TestNg.xml and updated maven dependency
</commit_message>
<xml_diff>
--- a/MyDemoProjectCBC/testData/testData.xlsx
+++ b/MyDemoProjectCBC/testData/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\new\CBC-selenium\MyDemoProjectCBC\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF763A-D41A-4F04-A2C2-637F3D6032F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E70C9B-6A13-424B-BBA4-0A24AEA01470}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D6381636-6C5F-4602-9AA4-18037967B7C4}"/>
   </bookViews>
@@ -52,10 +52,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,14 +86,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,7 +432,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -430,7 +441,10 @@
       <c r="C2" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C07C580C-773A-4F36-BB08-77D266038EEA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>